<commit_message>
ID:OMS-REV-02-->update after complete reviews
</commit_message>
<xml_diff>
--- a/PM/OnlineMobileStore_Review.xlsx
+++ b/PM/OnlineMobileStore_Review.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Design</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Document</t>
   </si>
   <si>
-    <t>Review applicable</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -63,15 +60,6 @@
     <t>Document ID</t>
   </si>
   <si>
-    <t>Document Description</t>
-  </si>
-  <si>
-    <t>Document Category</t>
-  </si>
-  <si>
-    <t>Document Type</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -82,6 +70,64 @@
   </si>
   <si>
     <t>Due Date</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>OnlineMobileStore_PMP</t>
+  </si>
+  <si>
+    <t>Salma Mohamed</t>
+  </si>
+  <si>
+    <t>Salma Khaled</t>
+  </si>
+  <si>
+    <t>31/3/2024</t>
+  </si>
+  <si>
+    <t>The PMP document should include Change managment Process, Issue Managment Plan, Configuration Manamgment Plan, and
+Review &amp;  Approval Process</t>
+  </si>
+  <si>
+    <t>PM/OnlineMobileStore_CIL</t>
+  </si>
+  <si>
+    <t>OMS-REV-PMP-01</t>
+  </si>
+  <si>
+    <t>OMS-REV-CIL-02</t>
+  </si>
+  <si>
+    <t>Information ought to be present within the CIL table</t>
+  </si>
+  <si>
+    <t>OMS-REV-IMP-03</t>
+  </si>
+  <si>
+    <t>PM/OnlineMobileStore_IMP</t>
+  </si>
+  <si>
+    <t>SaLma Khaled</t>
+  </si>
+  <si>
+    <t>Sama Wagdy</t>
+  </si>
+  <si>
+    <t>No comments</t>
+  </si>
+  <si>
+    <t>OMS-REV-CHG-04</t>
+  </si>
+  <si>
+    <t>PM/OnlineMobileStore_Changes</t>
+  </si>
+  <si>
+    <t>Ghada Hassan</t>
+  </si>
+  <si>
+    <t>_</t>
   </si>
 </sst>
 </file>
@@ -117,47 +163,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -454,104 +481,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="10" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5">
+        <v>45326</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:I2">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",G2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",G2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Sheet2!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Sheet2!$E$1:$E$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:I2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -577,7 +640,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -588,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ID:OMS-REV-03-->update review SRS & old comments
update after review SRS and ensure old comments are applied to the associated files
</commit_message>
<xml_diff>
--- a/PM/OnlineMobileStore_Review.xlsx
+++ b/PM/OnlineMobileStore_Review.xlsx
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
ID:OMS-REV-04-->update after reviewing SRS
</commit_message>
<xml_diff>
--- a/PM/OnlineMobileStore_Review.xlsx
+++ b/PM/OnlineMobileStore_Review.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Design</t>
   </si>
@@ -150,15 +150,57 @@
   <si>
     <t>OMS-REV-CIL-07</t>
   </si>
+  <si>
+    <t>OMS-REV-SRS-08</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1-"Product Categories" should not be specified as Side Panel at the "Client Dashboard" section at the feature table.
+2-Modify "Cart", "Payment method", and "Summary" in "Front End Details" section to be at the same page.
+3-Modify "Summary" in "Front End Details" section to be a pop-up message.
+4-Add "remove item" and "edit quantity" features to the "Card module" in "Front End Details" section.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5-Add the previos point to the "Technical Requirements" section also.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+6-In req "OMS_SRS_ Hist_01" and "OMS_SRS_ Hist_02", change the "account dashboard" to "client dashboard".
+7-In req id "OMS_SRS_Core-B_07.01", remove "redirects to page" part, and modify the scenario related to "Summary page".
+8-In req "OMS_SRS_Core-B_07.03", modify "Transaction Faild" senario.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -502,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +558,7 @@
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="45.85546875" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -703,8 +745,32 @@
         <v>31</v>
       </c>
     </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="278.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5">
+        <v>45356</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>